<commit_message>
layered domoic model into MSE
</commit_message>
<xml_diff>
--- a/models/contamination/paper/tables/TableS1_depuration_rates.xlsx
+++ b/models/contamination/paper/tables/TableS1_depuration_rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/dungeness/models/contamination/paper/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3664CBA-0EB8-5842-AFA3-914CEA761C91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E577014-C5D6-E84E-8644-58A0D4B85B81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{5B266C4C-58C2-FC43-A0EC-AD16F5939EAA}"/>
+    <workbookView xWindow="24040" yWindow="1060" windowWidth="30260" windowHeight="20460" xr2:uid="{5B266C4C-58C2-FC43-A0EC-AD16F5939EAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <r>
       <t>Rock crab (</t>
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>Lund et al. 1997</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>Schultz et al. 2008;</t>
@@ -426,13 +423,25 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Crustaceans</t>
+  </si>
+  <si>
+    <t>Bivalves</t>
+  </si>
+  <si>
+    <t>No studies known</t>
+  </si>
+  <si>
+    <t>Phylogenetic analogs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -455,12 +464,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF2E2E2E"/>
-      <name val="Georgia"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -494,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -502,7 +505,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -519,9 +521,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DB3779F-F91B-BB42-8E91-F80C448B150A}">
-  <dimension ref="A2:C33"/>
+  <dimension ref="A2:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C28" sqref="A2:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,222 +860,238 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B17" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-    </row>
-    <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
         <v>32</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="B37" t="s">
         <v>15</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" ht="23" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>